<commit_message>
Added a few details
</commit_message>
<xml_diff>
--- a/Start_up list(with contact details).xlsx
+++ b/Start_up list(with contact details).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="600" windowWidth="20775" windowHeight="5835"/>
+    <workbookView xWindow="150" yWindow="615" windowWidth="28455" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1102,6 +1102,6 @@
     <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>